<commit_message>
updated solution to include impossible case; updated xlsx file as well
</commit_message>
<xml_diff>
--- a/322-coin-change/leetcode-322-coin-change.xlsx
+++ b/322-coin-change/leetcode-322-coin-change.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/027a9447a4579b34/Documents/devel/lc-sol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\RHEL9\home\vulpski\projects\leetcode\322-coin-change\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{33B3D8ED-2D46-4FF8-A144-069614CA2E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA1EBB82-78A8-44D0-A390-9344C97BC58A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7B40B6-E6D8-4739-B77D-1FA4285BC37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FCD05CCE-8025-4674-9DA7-D570B2130B1F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -193,22 +193,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>220579</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142870</xdr:rowOff>
+      <xdr:colOff>462661</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>145381</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>14391</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>113621</xdr:rowOff>
+      <xdr:colOff>150395</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>150493</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{063716FE-2DA1-A12B-F8DD-36ED09F070CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C489016-159F-9F8E-6B7D-C7DD41F446C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -224,8 +224,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4501816" y="1095370"/>
-          <a:ext cx="3463443" cy="1314277"/>
+          <a:off x="4743898" y="716881"/>
+          <a:ext cx="3357365" cy="2501665"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -557,7 +557,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>